<commit_message>
Segundo intento con menos variables
</commit_message>
<xml_diff>
--- a/modelo/speedcraft-casos.xlsx
+++ b/modelo/speedcraft-casos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="225" windowWidth="18915" windowHeight="8385" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="285" windowWidth="18915" windowHeight="8325" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Hoja5" sheetId="5" r:id="rId3"/>
     <sheet name="speedcraft-casos" sheetId="6" r:id="rId4"/>
     <sheet name="speedcraft-alm-cofre" sheetId="7" r:id="rId5"/>
+    <sheet name="sinhuevo" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="102">
   <si>
     <t>PAN</t>
   </si>
@@ -297,6 +298,33 @@
   </si>
   <si>
     <t>alm2-inv-leche</t>
+  </si>
+  <si>
+    <t>alm1-cacao</t>
+  </si>
+  <si>
+    <t>alm1-leche</t>
+  </si>
+  <si>
+    <t>alm1-trigo</t>
+  </si>
+  <si>
+    <t>cofre-galleta-cacao</t>
+  </si>
+  <si>
+    <t>cofre-galleta-leche</t>
+  </si>
+  <si>
+    <t>cofre-galleta-trigo</t>
+  </si>
+  <si>
+    <t>cofre-pan-cacao</t>
+  </si>
+  <si>
+    <t>cofre-pan-leche</t>
+  </si>
+  <si>
+    <t>cofre-pan-trigo</t>
   </si>
 </sst>
 </file>
@@ -7687,16 +7715,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:K5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" customWidth="1"/>
-    <col min="5" max="6" width="6.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
@@ -8195,4 +8225,258 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="38">
+        <v>15</v>
+      </c>
+      <c r="C2" s="38">
+        <v>20</v>
+      </c>
+      <c r="D2" s="38">
+        <v>30</v>
+      </c>
+      <c r="E2" s="41">
+        <v>0</v>
+      </c>
+      <c r="F2" s="41">
+        <v>0</v>
+      </c>
+      <c r="G2" s="41">
+        <v>0</v>
+      </c>
+      <c r="H2" s="41">
+        <v>0</v>
+      </c>
+      <c r="I2" s="43">
+        <v>0</v>
+      </c>
+      <c r="J2" s="43">
+        <v>0</v>
+      </c>
+      <c r="K2" s="43">
+        <v>0</v>
+      </c>
+      <c r="L2" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="33">
+        <v>15</v>
+      </c>
+      <c r="C3" s="33">
+        <v>20</v>
+      </c>
+      <c r="D3" s="33">
+        <v>20</v>
+      </c>
+      <c r="E3" s="36">
+        <v>0</v>
+      </c>
+      <c r="F3" s="36">
+        <v>0</v>
+      </c>
+      <c r="G3" s="36">
+        <v>0</v>
+      </c>
+      <c r="H3" s="36">
+        <v>0</v>
+      </c>
+      <c r="I3" s="28">
+        <v>0</v>
+      </c>
+      <c r="J3" s="28">
+        <v>0</v>
+      </c>
+      <c r="K3" s="28">
+        <v>0</v>
+      </c>
+      <c r="L3" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="38">
+        <v>15</v>
+      </c>
+      <c r="C4" s="38">
+        <v>15</v>
+      </c>
+      <c r="D4" s="38">
+        <v>20</v>
+      </c>
+      <c r="E4" s="41">
+        <v>0</v>
+      </c>
+      <c r="F4" s="41">
+        <v>0</v>
+      </c>
+      <c r="G4" s="41">
+        <v>0</v>
+      </c>
+      <c r="H4" s="41">
+        <v>0</v>
+      </c>
+      <c r="I4" s="43">
+        <v>5</v>
+      </c>
+      <c r="J4" s="43">
+        <v>0</v>
+      </c>
+      <c r="K4" s="43">
+        <v>0</v>
+      </c>
+      <c r="L4" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="33">
+        <v>5</v>
+      </c>
+      <c r="C5" s="33">
+        <v>15</v>
+      </c>
+      <c r="D5" s="33">
+        <v>20</v>
+      </c>
+      <c r="E5" s="36">
+        <v>0</v>
+      </c>
+      <c r="F5" s="36">
+        <v>5</v>
+      </c>
+      <c r="G5" s="36">
+        <v>0</v>
+      </c>
+      <c r="H5" s="36">
+        <v>0</v>
+      </c>
+      <c r="I5" s="28">
+        <v>5</v>
+      </c>
+      <c r="J5" s="28">
+        <v>0</v>
+      </c>
+      <c r="K5" s="28">
+        <v>0</v>
+      </c>
+      <c r="L5" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="33">
+        <v>5</v>
+      </c>
+      <c r="C6" s="33">
+        <v>15</v>
+      </c>
+      <c r="D6" s="33">
+        <v>10</v>
+      </c>
+      <c r="E6" s="36">
+        <v>5</v>
+      </c>
+      <c r="F6" s="36">
+        <v>0</v>
+      </c>
+      <c r="G6" s="36">
+        <v>0</v>
+      </c>
+      <c r="H6" s="36">
+        <v>0</v>
+      </c>
+      <c r="I6" s="28">
+        <v>5</v>
+      </c>
+      <c r="J6" s="28">
+        <v>0</v>
+      </c>
+      <c r="K6" s="28">
+        <v>0</v>
+      </c>
+      <c r="L6" s="28">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Crear las clases auxiliares para construir los casos
</commit_message>
<xml_diff>
--- a/modelo/speedcraft-casos.xlsx
+++ b/modelo/speedcraft-casos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="165" windowWidth="18915" windowHeight="8445" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="225" windowWidth="18915" windowHeight="8385" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -226,76 +226,76 @@
     <t>almacen2_leche</t>
   </si>
   <si>
-    <t>a-objetivo</t>
-  </si>
-  <si>
-    <t>cofre-pan</t>
-  </si>
-  <si>
-    <t>cofre-pan-ingr-trigo</t>
-  </si>
-  <si>
-    <t>cofre-pan-ingr-cacao</t>
-  </si>
-  <si>
-    <t>cofre-pan-ingr-huevo</t>
-  </si>
-  <si>
-    <t>cofre-pan-ingr-leche</t>
-  </si>
-  <si>
-    <t>cofre-galleta-ingr-trigo</t>
-  </si>
-  <si>
-    <t>cofre-galleta-ingr-cacao</t>
-  </si>
-  <si>
-    <t>cofre-galleta-ingr-huevo</t>
-  </si>
-  <si>
-    <t>cofre-galleta-ingr-leche</t>
-  </si>
-  <si>
-    <t>cofre-pastel-ingr-trigo</t>
-  </si>
-  <si>
-    <t>cofre-pastel-ingr-cacao</t>
-  </si>
-  <si>
-    <t>cofre-pastel-ingr-huevo</t>
-  </si>
-  <si>
-    <t>cofre-pastel-ingr-leche</t>
-  </si>
-  <si>
-    <t>cofre-galleta</t>
-  </si>
-  <si>
-    <t>cofre-pastel</t>
-  </si>
-  <si>
-    <t>alm1-inv-trigo</t>
-  </si>
-  <si>
-    <t>alm1-inv-cacao</t>
-  </si>
-  <si>
-    <t>alm1-inv-huevo</t>
-  </si>
-  <si>
-    <t>alm1-inv-leche</t>
-  </si>
-  <si>
-    <t>alm2-inv-trigo</t>
-  </si>
-  <si>
-    <t>alm2-inv-cacao</t>
-  </si>
-  <si>
-    <t>alm2-inv-huevo</t>
-  </si>
-  <si>
-    <t>alm2-inv-leche</t>
+    <t>a_objetivo</t>
+  </si>
+  <si>
+    <t>alm1_inv_cacao</t>
+  </si>
+  <si>
+    <t>alm1_inv_huevo</t>
+  </si>
+  <si>
+    <t>alm1_inv_leche</t>
+  </si>
+  <si>
+    <t>alm1_inv_trigo</t>
+  </si>
+  <si>
+    <t>alm2_inv_cacao</t>
+  </si>
+  <si>
+    <t>alm2_inv_huevo</t>
+  </si>
+  <si>
+    <t>alm2_inv_leche</t>
+  </si>
+  <si>
+    <t>alm2_inv_trigo</t>
+  </si>
+  <si>
+    <t>cofre_galleta</t>
+  </si>
+  <si>
+    <t>cofre_galleta_ingr_cacao</t>
+  </si>
+  <si>
+    <t>cofre_galleta_ingr_huevo</t>
+  </si>
+  <si>
+    <t>cofre_galleta_ingr_leche</t>
+  </si>
+  <si>
+    <t>cofre_galleta_ingr_trigo</t>
+  </si>
+  <si>
+    <t>cofre_pan</t>
+  </si>
+  <si>
+    <t>cofre_pan_ingr_cacao</t>
+  </si>
+  <si>
+    <t>cofre_pan_ingr_huevo</t>
+  </si>
+  <si>
+    <t>cofre_pan_ingr_leche</t>
+  </si>
+  <si>
+    <t>cofre_pan_ingr_trigo</t>
+  </si>
+  <si>
+    <t>cofre_pastel</t>
+  </si>
+  <si>
+    <t>cofre_pastel_ingr_cacao</t>
+  </si>
+  <si>
+    <t>cofre_pastel_ingr_huevo</t>
+  </si>
+  <si>
+    <t>cofre_pastel_ingr_leche</t>
+  </si>
+  <si>
+    <t>cofre_pastel_ingr_trigo</t>
   </si>
 </sst>
 </file>
@@ -5103,8 +5103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB19"/>
   <sheetViews>
-    <sheetView topLeftCell="M16" workbookViewId="0">
-      <selection sqref="A1:AB19"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6623,19 +6623,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5:X5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="7.140625" customWidth="1"/>
-    <col min="4" max="14" width="6.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" customWidth="1"/>
+    <col min="5" max="9" width="7.28515625" customWidth="1"/>
+    <col min="10" max="14" width="6.42578125" customWidth="1"/>
     <col min="15" max="15" width="10" customWidth="1"/>
     <col min="16" max="18" width="6.42578125" customWidth="1"/>
-    <col min="19" max="19" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.7109375" customWidth="1"/>
     <col min="20" max="24" width="6.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6644,73 +6646,73 @@
         <v>69</v>
       </c>
       <c r="B1" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="P1" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q1" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="R1" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="S1" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="T1" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" s="34" t="s">
+      <c r="U1" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="V1" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="W1" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="X1" s="26" t="s">
         <v>92</v>
-      </c>
-      <c r="I1" s="34" t="s">
-        <v>89</v>
-      </c>
-      <c r="J1" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="K1" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="L1" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="M1" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="N1" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="O1" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="P1" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q1" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="R1" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="S1" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="T1" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="U1" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="V1" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="W1" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="X1" s="26" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>